<commit_message>
Edit Burn Down Chart
</commit_message>
<xml_diff>
--- a/src/BurnDownChart.xlsx
+++ b/src/BurnDownChart.xlsx
@@ -108,12 +108,6 @@
     <t>Day 1</t>
   </si>
   <si>
-    <t>Story 4</t>
-  </si>
-  <si>
-    <t>Task 4.3</t>
-  </si>
-  <si>
     <t>Task 4.4</t>
   </si>
   <si>
@@ -187,6 +181,12 @@
   </si>
   <si>
     <t>Kegunaan Benchmark</t>
+  </si>
+  <si>
+    <t>Beberapa Aplikasi Android yang kami sarankan</t>
+  </si>
+  <si>
+    <t>5 Aplikasi Games yang kami sarankan</t>
   </si>
 </sst>
 </file>
@@ -511,19 +511,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,25 +533,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="58211328"/>
-        <c:axId val="60351232"/>
+        <c:axId val="38279424"/>
+        <c:axId val="55071488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58211328"/>
+        <c:axId val="38279424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60351232"/>
+        <c:crossAx val="55071488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60351232"/>
+        <c:axId val="55071488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +559,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58211328"/>
+        <c:crossAx val="38279424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -572,7 +572,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -901,7 +901,7 @@
   <dimension ref="A1:XFD58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -917,7 +917,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -33690,7 +33690,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -50111,10 +50111,10 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>4</v>
@@ -50154,13 +50154,13 @@
     <row r="6" spans="1:16384">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>
@@ -50195,13 +50195,13 @@
     <row r="7" spans="1:16384">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4">
         <v>2</v>
@@ -50236,13 +50236,13 @@
     <row r="8" spans="1:16384">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="4">
         <v>4</v>
@@ -50277,13 +50277,13 @@
     <row r="9" spans="1:16384">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" s="4">
         <v>4</v>
@@ -50318,13 +50318,13 @@
     <row r="10" spans="1:16384">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" s="4">
         <v>4</v>
@@ -50359,13 +50359,13 @@
     <row r="11" spans="1:16384">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" s="4">
         <v>6</v>
@@ -50400,13 +50400,13 @@
     <row r="12" spans="1:16384">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E12" s="4">
         <v>3</v>
@@ -50441,13 +50441,13 @@
     <row r="13" spans="1:16384">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4">
         <v>6</v>
@@ -50482,13 +50482,13 @@
     <row r="14" spans="1:16384">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" s="4">
         <v>6</v>
@@ -50523,13 +50523,13 @@
     <row r="15" spans="1:16384">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" s="4">
         <v>4</v>
@@ -50564,13 +50564,13 @@
     <row r="16" spans="1:16384">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -50605,13 +50605,13 @@
     <row r="17" spans="1:21">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -50646,13 +50646,13 @@
     <row r="18" spans="1:21">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="4">
         <v>10</v>
@@ -50687,13 +50687,13 @@
     <row r="19" spans="1:21">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E19" s="4">
         <v>8</v>
@@ -50728,13 +50728,13 @@
     <row r="20" spans="1:21">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E20" s="4">
         <v>9</v>
@@ -50769,7 +50769,7 @@
     <row r="21" spans="1:21">
       <c r="A21" s="1"/>
       <c r="B21" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -50833,7 +50833,7 @@
     <row r="22" spans="1:21">
       <c r="A22" s="1"/>
       <c r="B22" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -50842,24 +50842,24 @@
         <v>70</v>
       </c>
       <c r="F22" s="4">
+        <f>SUM(F6:F20)</f>
+        <v>64</v>
+      </c>
+      <c r="G22" s="4">
+        <f>SUM(G6:G20)</f>
+        <v>60</v>
+      </c>
+      <c r="H22" s="4">
         <f>SUM(H6:H20)</f>
         <v>51</v>
       </c>
-      <c r="G22" s="4">
+      <c r="I22" s="4">
         <f>SUM(I6:I20)</f>
         <v>46</v>
       </c>
-      <c r="H22" s="4">
+      <c r="J22" s="4">
         <f>SUM(J6:J20)</f>
         <v>39</v>
-      </c>
-      <c r="I22" s="4">
-        <f>SUM(K6:K20)</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="4">
-        <f>SUM(L6:L20)</f>
-        <v>0</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>

</xml_diff>

<commit_message>
Edit BurnDown & LogBook
</commit_message>
<xml_diff>
--- a/src/BurnDownChart.xlsx
+++ b/src/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
   <si>
     <t>Project</t>
   </si>
@@ -232,6 +232,27 @@
   </si>
   <si>
     <t>Tips Memilih Perangkat Android yang Asli atau Replika</t>
+  </si>
+  <si>
+    <t>Alasan Memilih android</t>
+  </si>
+  <si>
+    <t>Tips Memilih Android</t>
+  </si>
+  <si>
+    <t>Tips Android</t>
+  </si>
+  <si>
+    <t>Alasan memilih Android</t>
+  </si>
+  <si>
+    <t>Tambahan dari Beberapa Aplikasi yang kami sarankan</t>
+  </si>
+  <si>
+    <t>5 Aplikasi Android untuk menjadikan ponsel sebagai scanner tulisan</t>
+  </si>
+  <si>
+    <t>Aplikasi terbaik untuk keamanan android dan cara melacak perangkat android yang hilang</t>
   </si>
 </sst>
 </file>
@@ -467,40 +488,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>84.333333333333329</c:v>
+                  <c:v>91.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76.666666666666657</c:v>
+                  <c:v>83.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68.999999999999986</c:v>
+                  <c:v>75.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>61.333333333333321</c:v>
+                  <c:v>66.666666666666686</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53.666666666666657</c:v>
+                  <c:v>58.33333333333335</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45.999999999999993</c:v>
+                  <c:v>50.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38.333333333333329</c:v>
+                  <c:v>41.666666666666679</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.666666666666661</c:v>
+                  <c:v>33.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22.999999999999993</c:v>
+                  <c:v>25.000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.333333333333325</c:v>
+                  <c:v>16.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.6666666666666581</c:v>
+                  <c:v>8.3333333333333375</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-8.8817841970012523E-15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -576,31 +597,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>61</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -619,11 +640,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="57377152"/>
-        <c:axId val="57378688"/>
+        <c:axId val="76794112"/>
+        <c:axId val="76804096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57377152"/>
+        <c:axId val="76794112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,14 +661,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57378688"/>
+        <c:crossAx val="76804096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57378688"/>
+        <c:axId val="76804096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -655,7 +676,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57377152"/>
+        <c:crossAx val="76794112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -678,7 +699,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1006,15 +1027,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" s="5" customFormat="1" ht="15.75">
@@ -50295,7 +50316,9 @@
       <c r="M6" s="4">
         <v>0</v>
       </c>
-      <c r="N6" s="4"/>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
@@ -50342,7 +50365,9 @@
       <c r="M7" s="4">
         <v>0</v>
       </c>
-      <c r="N7" s="4"/>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
@@ -50389,7 +50414,9 @@
       <c r="M8" s="4">
         <v>0</v>
       </c>
-      <c r="N8" s="4"/>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -50436,7 +50463,9 @@
       <c r="M9" s="4">
         <v>0</v>
       </c>
-      <c r="N9" s="4"/>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
@@ -50483,7 +50512,9 @@
       <c r="M10" s="4">
         <v>0</v>
       </c>
-      <c r="N10" s="4"/>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -50530,7 +50561,9 @@
       <c r="M11" s="4">
         <v>0</v>
       </c>
-      <c r="N11" s="4"/>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
@@ -50577,7 +50610,9 @@
       <c r="M12" s="4">
         <v>0</v>
       </c>
-      <c r="N12" s="4"/>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
@@ -50624,7 +50659,9 @@
       <c r="M13" s="4">
         <v>0</v>
       </c>
-      <c r="N13" s="4"/>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
@@ -50671,7 +50708,9 @@
       <c r="M14" s="4">
         <v>0</v>
       </c>
-      <c r="N14" s="4"/>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
@@ -50718,7 +50757,9 @@
       <c r="M15" s="4">
         <v>0</v>
       </c>
-      <c r="N15" s="4"/>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
@@ -50765,7 +50806,9 @@
       <c r="M16" s="4">
         <v>0</v>
       </c>
-      <c r="N16" s="4"/>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
@@ -50812,7 +50855,9 @@
       <c r="M17" s="4">
         <v>0</v>
       </c>
-      <c r="N17" s="4"/>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
@@ -50859,7 +50904,9 @@
       <c r="M18" s="4">
         <v>0</v>
       </c>
-      <c r="N18" s="4"/>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
@@ -50906,7 +50953,9 @@
       <c r="M19" s="4">
         <v>0</v>
       </c>
-      <c r="N19" s="4"/>
+      <c r="N19" s="4">
+        <v>0</v>
+      </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
@@ -50953,7 +51002,9 @@
       <c r="M20" s="4">
         <v>0</v>
       </c>
-      <c r="N20" s="4"/>
+      <c r="N20" s="4">
+        <v>0</v>
+      </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
@@ -51000,7 +51051,9 @@
       <c r="M21" s="4">
         <v>0</v>
       </c>
-      <c r="N21" s="4"/>
+      <c r="N21" s="4">
+        <v>0</v>
+      </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
@@ -51047,7 +51100,9 @@
       <c r="M22" s="4">
         <v>1</v>
       </c>
-      <c r="N22" s="4"/>
+      <c r="N22" s="4">
+        <v>0</v>
+      </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
@@ -51094,7 +51149,9 @@
       <c r="M23" s="4">
         <v>1</v>
       </c>
-      <c r="N23" s="4"/>
+      <c r="N23" s="4">
+        <v>0</v>
+      </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
@@ -51141,7 +51198,9 @@
       <c r="M24" s="4">
         <v>1</v>
       </c>
-      <c r="N24" s="4"/>
+      <c r="N24" s="4">
+        <v>0</v>
+      </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
@@ -51188,7 +51247,9 @@
       <c r="M25" s="4">
         <v>1</v>
       </c>
-      <c r="N25" s="4"/>
+      <c r="N25" s="4">
+        <v>0</v>
+      </c>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
@@ -51235,7 +51296,9 @@
       <c r="M26" s="4">
         <v>1</v>
       </c>
-      <c r="N26" s="4"/>
+      <c r="N26" s="4">
+        <v>0</v>
+      </c>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
@@ -51282,7 +51345,9 @@
       <c r="M27" s="4">
         <v>1</v>
       </c>
-      <c r="N27" s="4"/>
+      <c r="N27" s="4">
+        <v>0</v>
+      </c>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
@@ -51329,7 +51394,9 @@
       <c r="M28" s="4">
         <v>2</v>
       </c>
-      <c r="N28" s="4"/>
+      <c r="N28" s="4">
+        <v>0</v>
+      </c>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
@@ -51376,7 +51443,9 @@
       <c r="M29" s="4">
         <v>1</v>
       </c>
-      <c r="N29" s="4"/>
+      <c r="N29" s="4">
+        <v>0</v>
+      </c>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
@@ -51423,7 +51492,9 @@
       <c r="M30" s="4">
         <v>3</v>
       </c>
-      <c r="N30" s="4"/>
+      <c r="N30" s="4">
+        <v>0</v>
+      </c>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
@@ -51470,7 +51541,9 @@
       <c r="M31" s="4">
         <v>1</v>
       </c>
-      <c r="N31" s="4"/>
+      <c r="N31" s="4">
+        <v>0</v>
+      </c>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
@@ -51517,7 +51590,9 @@
       <c r="M32" s="4">
         <v>2</v>
       </c>
-      <c r="N32" s="4"/>
+      <c r="N32" s="4">
+        <v>0</v>
+      </c>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
@@ -51564,7 +51639,9 @@
       <c r="M33" s="4">
         <v>3</v>
       </c>
-      <c r="N33" s="4"/>
+      <c r="N33" s="4">
+        <v>0</v>
+      </c>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
@@ -51578,18 +51655,42 @@
       <c r="B34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
+      <c r="C34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="4">
+        <v>3</v>
+      </c>
+      <c r="F34" s="4">
+        <v>3</v>
+      </c>
+      <c r="G34" s="4">
+        <v>3</v>
+      </c>
+      <c r="H34" s="4">
+        <v>3</v>
+      </c>
+      <c r="I34" s="4">
+        <v>3</v>
+      </c>
+      <c r="J34" s="4">
+        <v>3</v>
+      </c>
+      <c r="K34" s="4">
+        <v>3</v>
+      </c>
+      <c r="L34" s="4">
+        <v>3</v>
+      </c>
+      <c r="M34" s="4">
+        <v>3</v>
+      </c>
+      <c r="N34" s="4">
+        <v>3</v>
+      </c>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
@@ -51603,18 +51704,42 @@
       <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
+      <c r="C35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="4">
+        <v>1</v>
+      </c>
+      <c r="F35" s="4">
+        <v>1</v>
+      </c>
+      <c r="G35" s="4">
+        <v>1</v>
+      </c>
+      <c r="H35" s="4">
+        <v>1</v>
+      </c>
+      <c r="I35" s="4">
+        <v>1</v>
+      </c>
+      <c r="J35" s="4">
+        <v>1</v>
+      </c>
+      <c r="K35" s="4">
+        <v>1</v>
+      </c>
+      <c r="L35" s="4">
+        <v>1</v>
+      </c>
+      <c r="M35" s="4">
+        <v>1</v>
+      </c>
+      <c r="N35" s="4">
+        <v>1</v>
+      </c>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
@@ -51628,18 +51753,42 @@
       <c r="B36" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
+      <c r="C36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2</v>
+      </c>
+      <c r="F36" s="4">
+        <v>2</v>
+      </c>
+      <c r="G36" s="4">
+        <v>2</v>
+      </c>
+      <c r="H36" s="4">
+        <v>2</v>
+      </c>
+      <c r="I36" s="4">
+        <v>2</v>
+      </c>
+      <c r="J36" s="4">
+        <v>2</v>
+      </c>
+      <c r="K36" s="4">
+        <v>2</v>
+      </c>
+      <c r="L36" s="4">
+        <v>2</v>
+      </c>
+      <c r="M36" s="4">
+        <v>2</v>
+      </c>
+      <c r="N36" s="4">
+        <v>2</v>
+      </c>
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
@@ -51653,18 +51802,42 @@
       <c r="B37" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
+      <c r="C37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="4">
+        <v>2</v>
+      </c>
+      <c r="F37" s="4">
+        <v>2</v>
+      </c>
+      <c r="G37" s="4">
+        <v>2</v>
+      </c>
+      <c r="H37" s="4">
+        <v>2</v>
+      </c>
+      <c r="I37" s="4">
+        <v>2</v>
+      </c>
+      <c r="J37" s="4">
+        <v>2</v>
+      </c>
+      <c r="K37" s="4">
+        <v>2</v>
+      </c>
+      <c r="L37" s="4">
+        <v>2</v>
+      </c>
+      <c r="M37" s="4">
+        <v>2</v>
+      </c>
+      <c r="N37" s="4">
+        <v>2</v>
+      </c>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
@@ -51856,56 +52029,56 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="4">
-        <f>SUM(E6:E33)</f>
-        <v>92</v>
+        <f>SUM(E6:E37)</f>
+        <v>100</v>
       </c>
       <c r="F45" s="4">
         <f>E45-$E$45/12</f>
-        <v>84.333333333333329</v>
+        <v>91.666666666666671</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" ref="G45:Q45" si="0">F45-$E$45/12</f>
-        <v>76.666666666666657</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="H45" s="4">
         <f>G45-$E$45/12</f>
-        <v>68.999999999999986</v>
+        <v>75.000000000000014</v>
       </c>
       <c r="I45" s="4">
         <f t="shared" si="0"/>
-        <v>61.333333333333321</v>
+        <v>66.666666666666686</v>
       </c>
       <c r="J45" s="4">
         <f t="shared" si="0"/>
-        <v>53.666666666666657</v>
+        <v>58.33333333333335</v>
       </c>
       <c r="K45" s="4">
         <f t="shared" si="0"/>
-        <v>45.999999999999993</v>
+        <v>50.000000000000014</v>
       </c>
       <c r="L45" s="4">
         <f t="shared" si="0"/>
-        <v>38.333333333333329</v>
+        <v>41.666666666666679</v>
       </c>
       <c r="M45" s="4">
         <f t="shared" si="0"/>
-        <v>30.666666666666661</v>
+        <v>33.333333333333343</v>
       </c>
       <c r="N45" s="4">
         <f>M45-$E$45/12</f>
-        <v>22.999999999999993</v>
+        <v>25.000000000000007</v>
       </c>
       <c r="O45" s="4">
         <f t="shared" si="0"/>
-        <v>15.333333333333325</v>
+        <v>16.666666666666671</v>
       </c>
       <c r="P45" s="4">
         <f t="shared" si="0"/>
-        <v>7.6666666666666581</v>
+        <v>8.3333333333333375</v>
       </c>
       <c r="Q45" s="4">
         <f t="shared" si="0"/>
-        <v>-8.8817841970012523E-15</v>
+        <v>0</v>
       </c>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
@@ -51921,43 +52094,43 @@
       <c r="D46" s="7"/>
       <c r="E46" s="4">
         <f t="shared" ref="E46:Q46" si="1">SUM(E6:E44)</f>
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F46" s="4">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="H46" s="4">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="I46" s="4">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="J46" s="4">
         <f t="shared" si="1"/>
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="K46" s="4">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="L46" s="4">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="M46" s="4">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="N46" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O46" s="4">
         <f t="shared" si="1"/>

</xml_diff>